<commit_message>
Increment the version number for any new changes/fixes which are made (v0.1.3)
</commit_message>
<xml_diff>
--- a/dvk-som-pinout.xlsx
+++ b/dvk-som-pinout.xlsx
@@ -2208,7 +2208,7 @@
     <t xml:space="preserve">P4.03</t>
   </si>
   <si>
-    <t xml:space="preserve">MUTE (was SPDIF_TX)</t>
+    <t xml:space="preserve">nMUTE (was SPDIF_TX)</t>
   </si>
   <si>
     <t xml:space="preserve">F6</t>
@@ -2320,6 +2320,7 @@
         <sz val="10"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(protos using </t>
     </r>
@@ -3863,7 +3864,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3923,11 +3924,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">

</xml_diff>

<commit_message>
Since MISO/MOSI are correct on the upcoming prototypes then there's no need to point out the old error in the pinout spreadsheet, remove this remark in the spreadsheet
</commit_message>
<xml_diff>
--- a/dvk-som-pinout.xlsx
+++ b/dvk-som-pinout.xlsx
@@ -2283,8 +2283,7 @@
     <t xml:space="preserve">P4.65</t>
   </si>
   <si>
-    <t xml:space="preserve">ECSPI1_MOSI
-(protos using MISO!!!)</t>
+    <t xml:space="preserve">ECSPI1_MOSI</t>
   </si>
   <si>
     <t xml:space="preserve">A4</t>
@@ -2305,34 +2304,7 @@
     <t xml:space="preserve">P4.51</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve">ECSPI1_MISO
-(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">(protos using </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve">MOSI!!!)</t>
-    </r>
+    <t xml:space="preserve">ECSPI1_MISO</t>
   </si>
   <si>
     <t xml:space="preserve">B4</t>
@@ -3926,7 +3898,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3943,12 +3915,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFF200"/>
         <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFED1C24"/>
-        <bgColor rgb="FF993300"/>
       </patternFill>
     </fill>
   </fills>
@@ -4082,7 +4048,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4120,7 +4086,7 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFED1C24"/>
+      <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFF200"/>
@@ -7281,7 +7247,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="103" s="10" customFormat="true" ht="21.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" s="10" customFormat="true" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="9" t="s">
         <v>672</v>
       </c>
@@ -7311,7 +7277,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="104" s="10" customFormat="true" ht="21.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" s="10" customFormat="true" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="9" t="s">
         <v>679</v>
       </c>

</xml_diff>

<commit_message>
Color the pins orange and dark-orange in the pinout spreadsheet for the pins which would critically conflict with EmCraft's basebaord device tree (resulting in an output connected to an output)
</commit_message>
<xml_diff>
--- a/dvk-som-pinout.xlsx
+++ b/dvk-som-pinout.xlsx
@@ -199,7 +199,7 @@
     <t xml:space="preserve">P3.21</t>
   </si>
   <si>
-    <t xml:space="preserve">DSI_BL_PWM (was GPIO1_IO01)</t>
+    <t xml:space="preserve">DSI_BL_PWM (GPIO1_IO01)</t>
   </si>
   <si>
     <t xml:space="preserve">T7</t>
@@ -969,7 +969,7 @@
     <t xml:space="preserve">P1.56</t>
   </si>
   <si>
-    <t xml:space="preserve">WIFI_WAKE (was SD2_WP)</t>
+    <t xml:space="preserve">WIFI_WAKE (was SD_WAKE/SD2_WP)</t>
   </si>
   <si>
     <t xml:space="preserve">M21</t>
@@ -3898,7 +3898,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3915,6 +3915,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFF200"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF58220"/>
+        <bgColor rgb="FFFAA61A"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFAA61A"/>
+        <bgColor rgb="FFF58220"/>
       </patternFill>
     </fill>
   </fills>
@@ -3963,7 +3975,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4028,6 +4040,10 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4036,11 +4052,19 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4128,8 +4152,8 @@
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FFFAA61A"/>
+      <rgbColor rgb="FFF58220"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
@@ -4469,7 +4493,7 @@
       <c r="A12" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="6" t="s">
         <v>58</v>
       </c>
       <c r="C12" s="7" t="s">
@@ -5509,11 +5533,11 @@
       </c>
       <c r="L47" s="7"/>
     </row>
-    <row r="48" s="10" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="48" s="10" customFormat="true" ht="21.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="7" t="s">
         <v>285</v>
       </c>
-      <c r="B48" s="12" t="s">
+      <c r="B48" s="6" t="s">
         <v>286</v>
       </c>
       <c r="C48" s="7" t="s">
@@ -5983,7 +6007,7 @@
       <c r="A64" s="7" t="s">
         <v>392</v>
       </c>
-      <c r="B64" s="16" t="s">
+      <c r="B64" s="17" t="s">
         <v>393</v>
       </c>
       <c r="C64" s="7" t="s">
@@ -6011,7 +6035,7 @@
       <c r="A65" s="7" t="s">
         <v>398</v>
       </c>
-      <c r="B65" s="17" t="s">
+      <c r="B65" s="18" t="s">
         <v>399</v>
       </c>
       <c r="C65" s="7" t="s">
@@ -6039,7 +6063,7 @@
       <c r="A66" s="7" t="s">
         <v>404</v>
       </c>
-      <c r="B66" s="17" t="s">
+      <c r="B66" s="18" t="s">
         <v>405</v>
       </c>
       <c r="C66" s="7" t="s">
@@ -6071,7 +6095,7 @@
       <c r="A67" s="7" t="s">
         <v>412</v>
       </c>
-      <c r="B67" s="17" t="s">
+      <c r="B67" s="18" t="s">
         <v>413</v>
       </c>
       <c r="C67" s="7" t="s">
@@ -6103,7 +6127,7 @@
       <c r="A68" s="7" t="s">
         <v>419</v>
       </c>
-      <c r="B68" s="17" t="s">
+      <c r="B68" s="18" t="s">
         <v>420</v>
       </c>
       <c r="C68" s="7" t="s">
@@ -6135,7 +6159,7 @@
       <c r="A69" s="7" t="s">
         <v>426</v>
       </c>
-      <c r="B69" s="16" t="s">
+      <c r="B69" s="19" t="s">
         <v>427</v>
       </c>
       <c r="C69" s="7" t="s">
@@ -6167,7 +6191,7 @@
       <c r="A70" s="5" t="s">
         <v>434</v>
       </c>
-      <c r="B70" s="18" t="s">
+      <c r="B70" s="20" t="s">
         <v>435</v>
       </c>
       <c r="C70" s="7" t="s">
@@ -6199,7 +6223,7 @@
       <c r="A71" s="5" t="s">
         <v>441</v>
       </c>
-      <c r="B71" s="18" t="s">
+      <c r="B71" s="20" t="s">
         <v>442</v>
       </c>
       <c r="C71" s="7" t="s">
@@ -6231,7 +6255,7 @@
       <c r="A72" s="5" t="s">
         <v>448</v>
       </c>
-      <c r="B72" s="18" t="s">
+      <c r="B72" s="20" t="s">
         <v>449</v>
       </c>
       <c r="C72" s="7" t="s">
@@ -6265,7 +6289,7 @@
       <c r="A73" s="5" t="s">
         <v>456</v>
       </c>
-      <c r="B73" s="19" t="s">
+      <c r="B73" s="21" t="s">
         <v>457</v>
       </c>
       <c r="C73" s="7" t="s">
@@ -6299,7 +6323,7 @@
       <c r="A74" s="5" t="s">
         <v>464</v>
       </c>
-      <c r="B74" s="19" t="s">
+      <c r="B74" s="21" t="s">
         <v>465</v>
       </c>
       <c r="C74" s="7" t="s">
@@ -6333,7 +6357,7 @@
       <c r="A75" s="5" t="s">
         <v>472</v>
       </c>
-      <c r="B75" s="19" t="s">
+      <c r="B75" s="21" t="s">
         <v>473</v>
       </c>
       <c r="C75" s="7" t="s">
@@ -6367,7 +6391,7 @@
       <c r="A76" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="B76" s="18" t="s">
+      <c r="B76" s="20" t="s">
         <v>481</v>
       </c>
       <c r="C76" s="7" t="s">
@@ -6403,7 +6427,7 @@
       <c r="A77" s="5" t="s">
         <v>490</v>
       </c>
-      <c r="B77" s="18" t="s">
+      <c r="B77" s="20" t="s">
         <v>491</v>
       </c>
       <c r="C77" s="7" t="s">
@@ -6441,7 +6465,7 @@
       <c r="A78" s="5" t="s">
         <v>500</v>
       </c>
-      <c r="B78" s="18" t="s">
+      <c r="B78" s="22" t="s">
         <v>501</v>
       </c>
       <c r="C78" s="7" t="s">
@@ -6477,7 +6501,7 @@
       <c r="A79" s="5" t="s">
         <v>510</v>
       </c>
-      <c r="B79" s="18" t="s">
+      <c r="B79" s="20" t="s">
         <v>511</v>
       </c>
       <c r="C79" s="7" t="s">
@@ -6515,7 +6539,7 @@
       <c r="A80" s="5" t="s">
         <v>519</v>
       </c>
-      <c r="B80" s="18" t="s">
+      <c r="B80" s="20" t="s">
         <v>520</v>
       </c>
       <c r="C80" s="7" t="s">
@@ -6547,7 +6571,7 @@
       <c r="A81" s="5" t="s">
         <v>525</v>
       </c>
-      <c r="B81" s="18" t="s">
+      <c r="B81" s="20" t="s">
         <v>526</v>
       </c>
       <c r="C81" s="7" t="s">
@@ -6579,7 +6603,7 @@
       <c r="A82" s="5" t="s">
         <v>531</v>
       </c>
-      <c r="B82" s="19" t="s">
+      <c r="B82" s="21" t="s">
         <v>532</v>
       </c>
       <c r="C82" s="7" t="s">
@@ -6613,7 +6637,7 @@
       <c r="A83" s="5" t="s">
         <v>538</v>
       </c>
-      <c r="B83" s="19" t="s">
+      <c r="B83" s="21" t="s">
         <v>539</v>
       </c>
       <c r="C83" s="7" t="s">
@@ -6647,7 +6671,7 @@
       <c r="A84" s="5" t="s">
         <v>546</v>
       </c>
-      <c r="B84" s="19" t="s">
+      <c r="B84" s="21" t="s">
         <v>547</v>
       </c>
       <c r="C84" s="7" t="s">
@@ -6681,7 +6705,7 @@
       <c r="A85" s="5" t="s">
         <v>554</v>
       </c>
-      <c r="B85" s="19" t="s">
+      <c r="B85" s="21" t="s">
         <v>555</v>
       </c>
       <c r="C85" s="7" t="s">
@@ -6715,7 +6739,7 @@
       <c r="A86" s="5" t="s">
         <v>562</v>
       </c>
-      <c r="B86" s="18" t="s">
+      <c r="B86" s="22" t="s">
         <v>563</v>
       </c>
       <c r="C86" s="7" t="s">
@@ -6751,7 +6775,7 @@
       <c r="A87" s="5" t="s">
         <v>569</v>
       </c>
-      <c r="B87" s="18" t="s">
+      <c r="B87" s="22" t="s">
         <v>570</v>
       </c>
       <c r="C87" s="7" t="s">
@@ -6787,7 +6811,7 @@
       <c r="A88" s="5" t="s">
         <v>576</v>
       </c>
-      <c r="B88" s="19" t="s">
+      <c r="B88" s="21" t="s">
         <v>577</v>
       </c>
       <c r="C88" s="7" t="s">
@@ -6823,7 +6847,7 @@
       <c r="A89" s="5" t="s">
         <v>584</v>
       </c>
-      <c r="B89" s="19" t="s">
+      <c r="B89" s="21" t="s">
         <v>585</v>
       </c>
       <c r="C89" s="7" t="s">
@@ -6857,7 +6881,7 @@
       <c r="A90" s="5" t="s">
         <v>592</v>
       </c>
-      <c r="B90" s="18" t="s">
+      <c r="B90" s="20" t="s">
         <v>593</v>
       </c>
       <c r="C90" s="7" t="s">
@@ -6889,7 +6913,7 @@
       <c r="A91" s="5" t="s">
         <v>598</v>
       </c>
-      <c r="B91" s="20" t="s">
+      <c r="B91" s="23" t="s">
         <v>599</v>
       </c>
       <c r="C91" s="7" t="s">
@@ -6919,7 +6943,7 @@
       <c r="A92" s="5" t="s">
         <v>604</v>
       </c>
-      <c r="B92" s="20" t="s">
+      <c r="B92" s="23" t="s">
         <v>605</v>
       </c>
       <c r="C92" s="7" t="s">
@@ -6949,7 +6973,7 @@
       <c r="A93" s="5" t="s">
         <v>610</v>
       </c>
-      <c r="B93" s="20" t="s">
+      <c r="B93" s="23" t="s">
         <v>611</v>
       </c>
       <c r="C93" s="7" t="s">
@@ -6979,7 +7003,7 @@
       <c r="A94" s="5" t="s">
         <v>616</v>
       </c>
-      <c r="B94" s="20" t="s">
+      <c r="B94" s="23" t="s">
         <v>617</v>
       </c>
       <c r="C94" s="7" t="s">
@@ -7009,7 +7033,7 @@
       <c r="A95" s="5" t="s">
         <v>622</v>
       </c>
-      <c r="B95" s="20" t="s">
+      <c r="B95" s="23" t="s">
         <v>623</v>
       </c>
       <c r="C95" s="7" t="s">
@@ -7039,7 +7063,7 @@
       <c r="A96" s="5" t="s">
         <v>628</v>
       </c>
-      <c r="B96" s="20" t="s">
+      <c r="B96" s="23" t="s">
         <v>629</v>
       </c>
       <c r="C96" s="7" t="s">
@@ -7069,7 +7093,7 @@
       <c r="A97" s="5" t="s">
         <v>634</v>
       </c>
-      <c r="B97" s="20" t="s">
+      <c r="B97" s="23" t="s">
         <v>635</v>
       </c>
       <c r="C97" s="7" t="s">
@@ -7099,7 +7123,7 @@
       <c r="A98" s="5" t="s">
         <v>640</v>
       </c>
-      <c r="B98" s="20" t="s">
+      <c r="B98" s="23" t="s">
         <v>641</v>
       </c>
       <c r="C98" s="7" t="s">
@@ -7131,7 +7155,7 @@
       <c r="A99" s="5" t="s">
         <v>647</v>
       </c>
-      <c r="B99" s="18" t="s">
+      <c r="B99" s="20" t="s">
         <v>648</v>
       </c>
       <c r="C99" s="7" t="s">
@@ -7161,7 +7185,7 @@
       <c r="A100" s="5" t="s">
         <v>653</v>
       </c>
-      <c r="B100" s="18" t="s">
+      <c r="B100" s="20" t="s">
         <v>654</v>
       </c>
       <c r="C100" s="7" t="s">
@@ -7191,7 +7215,7 @@
       <c r="A101" s="5" t="s">
         <v>659</v>
       </c>
-      <c r="B101" s="18" t="s">
+      <c r="B101" s="20" t="s">
         <v>660</v>
       </c>
       <c r="C101" s="7" t="s">
@@ -7251,7 +7275,7 @@
       <c r="A103" s="9" t="s">
         <v>672</v>
       </c>
-      <c r="B103" s="21" t="s">
+      <c r="B103" s="24" t="s">
         <v>673</v>
       </c>
       <c r="C103" s="7" t="s">
@@ -7281,7 +7305,7 @@
       <c r="A104" s="9" t="s">
         <v>679</v>
       </c>
-      <c r="B104" s="21" t="s">
+      <c r="B104" s="24" t="s">
         <v>680</v>
       </c>
       <c r="C104" s="7" t="s">
@@ -7706,7 +7730,7 @@
       </c>
     </row>
     <row r="118" s="10" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A118" s="22" t="s">
+      <c r="A118" s="25" t="s">
         <v>775</v>
       </c>
       <c r="B118" s="14" t="s">
@@ -7736,7 +7760,7 @@
       </c>
     </row>
     <row r="119" s="10" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A119" s="22" t="s">
+      <c r="A119" s="25" t="s">
         <v>782</v>
       </c>
       <c r="B119" s="14" t="s">
@@ -8203,7 +8227,7 @@
       <c r="A139" s="9" t="s">
         <v>853</v>
       </c>
-      <c r="B139" s="23" t="s">
+      <c r="B139" s="26" t="s">
         <v>854</v>
       </c>
       <c r="C139" s="7" t="s">
@@ -8225,7 +8249,7 @@
       <c r="A140" s="9" t="s">
         <v>856</v>
       </c>
-      <c r="B140" s="23" t="s">
+      <c r="B140" s="26" t="s">
         <v>857</v>
       </c>
       <c r="C140" s="7" t="s">
@@ -8247,7 +8271,7 @@
       <c r="A141" s="9" t="s">
         <v>859</v>
       </c>
-      <c r="B141" s="23" t="s">
+      <c r="B141" s="26" t="s">
         <v>860</v>
       </c>
       <c r="C141" s="7" t="s">
@@ -8269,7 +8293,7 @@
       <c r="A142" s="9" t="s">
         <v>862</v>
       </c>
-      <c r="B142" s="23" t="s">
+      <c r="B142" s="26" t="s">
         <v>863</v>
       </c>
       <c r="C142" s="7" t="s">
@@ -8291,7 +8315,7 @@
       <c r="A143" s="9" t="s">
         <v>865</v>
       </c>
-      <c r="B143" s="23" t="s">
+      <c r="B143" s="26" t="s">
         <v>866</v>
       </c>
       <c r="C143" s="7" t="s">
@@ -8995,7 +9019,7 @@
       <c r="A175" s="9" t="s">
         <v>961</v>
       </c>
-      <c r="B175" s="23" t="s">
+      <c r="B175" s="26" t="s">
         <v>962</v>
       </c>
       <c r="C175" s="7" t="s">
@@ -9017,7 +9041,7 @@
       <c r="A176" s="9" t="s">
         <v>964</v>
       </c>
-      <c r="B176" s="23" t="s">
+      <c r="B176" s="26" t="s">
         <v>965</v>
       </c>
       <c r="C176" s="7" t="s">
@@ -9039,7 +9063,7 @@
       <c r="A177" s="9" t="s">
         <v>967</v>
       </c>
-      <c r="B177" s="23" t="s">
+      <c r="B177" s="26" t="s">
         <v>968</v>
       </c>
       <c r="C177" s="7" t="s">
@@ -9801,7 +9825,7 @@
       <c r="A214" s="7" t="s">
         <v>1028</v>
       </c>
-      <c r="B214" s="24" t="s">
+      <c r="B214" s="27" t="s">
         <v>1029</v>
       </c>
       <c r="C214" s="7"/>
@@ -9821,7 +9845,7 @@
       <c r="A215" s="7" t="s">
         <v>1030</v>
       </c>
-      <c r="B215" s="25" t="s">
+      <c r="B215" s="28" t="s">
         <v>1031</v>
       </c>
       <c r="C215" s="7"/>
@@ -9841,7 +9865,7 @@
       <c r="A216" s="7" t="s">
         <v>1032</v>
       </c>
-      <c r="B216" s="25" t="s">
+      <c r="B216" s="28" t="s">
         <v>1033</v>
       </c>
       <c r="C216" s="7"/>
@@ -9861,7 +9885,7 @@
       <c r="A217" s="7" t="s">
         <v>1034</v>
       </c>
-      <c r="B217" s="25" t="s">
+      <c r="B217" s="28" t="s">
         <v>1035</v>
       </c>
       <c r="C217" s="7"/>
@@ -9881,7 +9905,7 @@
       <c r="A218" s="7" t="s">
         <v>1036</v>
       </c>
-      <c r="B218" s="25" t="s">
+      <c r="B218" s="28" t="s">
         <v>1035</v>
       </c>
       <c r="C218" s="7"/>
@@ -9901,7 +9925,7 @@
       <c r="A219" s="7" t="s">
         <v>1037</v>
       </c>
-      <c r="B219" s="25" t="s">
+      <c r="B219" s="28" t="s">
         <v>1035</v>
       </c>
       <c r="C219" s="7"/>
@@ -9925,7 +9949,7 @@
         <v>1039</v>
       </c>
       <c r="C220" s="7"/>
-      <c r="D220" s="26" t="s">
+      <c r="D220" s="29" t="s">
         <v>1002</v>
       </c>
       <c r="E220" s="7"/>
@@ -9941,7 +9965,7 @@
       <c r="A221" s="7" t="s">
         <v>1040</v>
       </c>
-      <c r="B221" s="25" t="s">
+      <c r="B221" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C221" s="7"/>
@@ -9961,7 +9985,7 @@
       <c r="A222" s="7" t="s">
         <v>1042</v>
       </c>
-      <c r="B222" s="25" t="s">
+      <c r="B222" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C222" s="7"/>
@@ -9981,7 +10005,7 @@
       <c r="A223" s="7" t="s">
         <v>1043</v>
       </c>
-      <c r="B223" s="25" t="s">
+      <c r="B223" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C223" s="7"/>
@@ -10001,7 +10025,7 @@
       <c r="A224" s="7" t="s">
         <v>1044</v>
       </c>
-      <c r="B224" s="25" t="s">
+      <c r="B224" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C224" s="7"/>
@@ -10021,7 +10045,7 @@
       <c r="A225" s="7" t="s">
         <v>1045</v>
       </c>
-      <c r="B225" s="25" t="s">
+      <c r="B225" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C225" s="7"/>
@@ -10041,7 +10065,7 @@
       <c r="A226" s="7" t="s">
         <v>1046</v>
       </c>
-      <c r="B226" s="25" t="s">
+      <c r="B226" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C226" s="7"/>
@@ -10061,7 +10085,7 @@
       <c r="A227" s="7" t="s">
         <v>1047</v>
       </c>
-      <c r="B227" s="25" t="s">
+      <c r="B227" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C227" s="7"/>
@@ -10081,7 +10105,7 @@
       <c r="A228" s="7" t="s">
         <v>1048</v>
       </c>
-      <c r="B228" s="25" t="s">
+      <c r="B228" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C228" s="7"/>
@@ -10101,7 +10125,7 @@
       <c r="A229" s="7" t="s">
         <v>1049</v>
       </c>
-      <c r="B229" s="25" t="s">
+      <c r="B229" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C229" s="7"/>
@@ -10121,7 +10145,7 @@
       <c r="A230" s="7" t="s">
         <v>1050</v>
       </c>
-      <c r="B230" s="25" t="s">
+      <c r="B230" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C230" s="7"/>
@@ -10141,7 +10165,7 @@
       <c r="A231" s="7" t="s">
         <v>1051</v>
       </c>
-      <c r="B231" s="25" t="s">
+      <c r="B231" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C231" s="7"/>
@@ -10161,7 +10185,7 @@
       <c r="A232" s="7" t="s">
         <v>1052</v>
       </c>
-      <c r="B232" s="25" t="s">
+      <c r="B232" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C232" s="7"/>
@@ -10181,7 +10205,7 @@
       <c r="A233" s="7" t="s">
         <v>1053</v>
       </c>
-      <c r="B233" s="25" t="s">
+      <c r="B233" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C233" s="7"/>
@@ -10201,7 +10225,7 @@
       <c r="A234" s="7" t="s">
         <v>1054</v>
       </c>
-      <c r="B234" s="25" t="s">
+      <c r="B234" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C234" s="7"/>
@@ -10221,7 +10245,7 @@
       <c r="A235" s="7" t="s">
         <v>1055</v>
       </c>
-      <c r="B235" s="25" t="s">
+      <c r="B235" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C235" s="7"/>
@@ -10241,7 +10265,7 @@
       <c r="A236" s="7" t="s">
         <v>1056</v>
       </c>
-      <c r="B236" s="25" t="s">
+      <c r="B236" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C236" s="7"/>
@@ -10261,7 +10285,7 @@
       <c r="A237" s="7" t="s">
         <v>1057</v>
       </c>
-      <c r="B237" s="25" t="s">
+      <c r="B237" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C237" s="7"/>
@@ -10281,7 +10305,7 @@
       <c r="A238" s="7" t="s">
         <v>1058</v>
       </c>
-      <c r="B238" s="25" t="s">
+      <c r="B238" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C238" s="7"/>
@@ -10301,7 +10325,7 @@
       <c r="A239" s="7" t="s">
         <v>1059</v>
       </c>
-      <c r="B239" s="25" t="s">
+      <c r="B239" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C239" s="7"/>
@@ -10321,7 +10345,7 @@
       <c r="A240" s="7" t="s">
         <v>1060</v>
       </c>
-      <c r="B240" s="25" t="s">
+      <c r="B240" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C240" s="7"/>
@@ -10341,7 +10365,7 @@
       <c r="A241" s="7" t="s">
         <v>1061</v>
       </c>
-      <c r="B241" s="25" t="s">
+      <c r="B241" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C241" s="7"/>
@@ -10361,7 +10385,7 @@
       <c r="A242" s="7" t="s">
         <v>1062</v>
       </c>
-      <c r="B242" s="25" t="s">
+      <c r="B242" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C242" s="7"/>
@@ -10381,7 +10405,7 @@
       <c r="A243" s="7" t="s">
         <v>1063</v>
       </c>
-      <c r="B243" s="25" t="s">
+      <c r="B243" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C243" s="7"/>
@@ -10401,7 +10425,7 @@
       <c r="A244" s="7" t="s">
         <v>1064</v>
       </c>
-      <c r="B244" s="25" t="s">
+      <c r="B244" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C244" s="7"/>
@@ -10421,7 +10445,7 @@
       <c r="A245" s="7" t="s">
         <v>1065</v>
       </c>
-      <c r="B245" s="25" t="s">
+      <c r="B245" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C245" s="7"/>
@@ -10441,7 +10465,7 @@
       <c r="A246" s="7" t="s">
         <v>1066</v>
       </c>
-      <c r="B246" s="25" t="s">
+      <c r="B246" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C246" s="7"/>
@@ -10461,7 +10485,7 @@
       <c r="A247" s="7" t="s">
         <v>1067</v>
       </c>
-      <c r="B247" s="25" t="s">
+      <c r="B247" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C247" s="7"/>
@@ -10481,7 +10505,7 @@
       <c r="A248" s="7" t="s">
         <v>1068</v>
       </c>
-      <c r="B248" s="25" t="s">
+      <c r="B248" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C248" s="7"/>
@@ -10501,7 +10525,7 @@
       <c r="A249" s="7" t="s">
         <v>1069</v>
       </c>
-      <c r="B249" s="25" t="s">
+      <c r="B249" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C249" s="7"/>
@@ -10521,7 +10545,7 @@
       <c r="A250" s="7" t="s">
         <v>1070</v>
       </c>
-      <c r="B250" s="25" t="s">
+      <c r="B250" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C250" s="7"/>
@@ -10541,7 +10565,7 @@
       <c r="A251" s="7" t="s">
         <v>1071</v>
       </c>
-      <c r="B251" s="25" t="s">
+      <c r="B251" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C251" s="7"/>
@@ -10561,7 +10585,7 @@
       <c r="A252" s="7" t="s">
         <v>1072</v>
       </c>
-      <c r="B252" s="25" t="s">
+      <c r="B252" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C252" s="7"/>
@@ -10581,7 +10605,7 @@
       <c r="A253" s="7" t="s">
         <v>1073</v>
       </c>
-      <c r="B253" s="25" t="s">
+      <c r="B253" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C253" s="7"/>
@@ -10601,7 +10625,7 @@
       <c r="A254" s="7" t="s">
         <v>1074</v>
       </c>
-      <c r="B254" s="25" t="s">
+      <c r="B254" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C254" s="7"/>
@@ -10621,7 +10645,7 @@
       <c r="A255" s="7" t="s">
         <v>1075</v>
       </c>
-      <c r="B255" s="25" t="s">
+      <c r="B255" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C255" s="7"/>
@@ -10641,7 +10665,7 @@
       <c r="A256" s="7" t="s">
         <v>1076</v>
       </c>
-      <c r="B256" s="25" t="s">
+      <c r="B256" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C256" s="7"/>
@@ -10661,7 +10685,7 @@
       <c r="A257" s="7" t="s">
         <v>1077</v>
       </c>
-      <c r="B257" s="25" t="s">
+      <c r="B257" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C257" s="7"/>
@@ -10681,7 +10705,7 @@
       <c r="A258" s="7" t="s">
         <v>1078</v>
       </c>
-      <c r="B258" s="25" t="s">
+      <c r="B258" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C258" s="7"/>
@@ -10701,7 +10725,7 @@
       <c r="A259" s="7" t="s">
         <v>1079</v>
       </c>
-      <c r="B259" s="25" t="s">
+      <c r="B259" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C259" s="7"/>
@@ -10721,7 +10745,7 @@
       <c r="A260" s="7" t="s">
         <v>1080</v>
       </c>
-      <c r="B260" s="25" t="s">
+      <c r="B260" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C260" s="7"/>
@@ -10741,7 +10765,7 @@
       <c r="A261" s="7" t="s">
         <v>1081</v>
       </c>
-      <c r="B261" s="25" t="s">
+      <c r="B261" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C261" s="7"/>
@@ -10761,7 +10785,7 @@
       <c r="A262" s="7" t="s">
         <v>1082</v>
       </c>
-      <c r="B262" s="25" t="s">
+      <c r="B262" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C262" s="7"/>
@@ -10781,7 +10805,7 @@
       <c r="A263" s="7" t="s">
         <v>1083</v>
       </c>
-      <c r="B263" s="25" t="s">
+      <c r="B263" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C263" s="7"/>
@@ -10801,7 +10825,7 @@
       <c r="A264" s="7" t="s">
         <v>1084</v>
       </c>
-      <c r="B264" s="25" t="s">
+      <c r="B264" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C264" s="7"/>
@@ -10821,7 +10845,7 @@
       <c r="A265" s="7" t="s">
         <v>1085</v>
       </c>
-      <c r="B265" s="25" t="s">
+      <c r="B265" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C265" s="7"/>
@@ -10841,7 +10865,7 @@
       <c r="A266" s="7" t="s">
         <v>1086</v>
       </c>
-      <c r="B266" s="25" t="s">
+      <c r="B266" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C266" s="7"/>
@@ -10861,7 +10885,7 @@
       <c r="A267" s="7" t="s">
         <v>1087</v>
       </c>
-      <c r="B267" s="25" t="s">
+      <c r="B267" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C267" s="7"/>
@@ -10881,7 +10905,7 @@
       <c r="A268" s="7" t="s">
         <v>1088</v>
       </c>
-      <c r="B268" s="25" t="s">
+      <c r="B268" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C268" s="7"/>
@@ -10901,7 +10925,7 @@
       <c r="A269" s="7" t="s">
         <v>1089</v>
       </c>
-      <c r="B269" s="25" t="s">
+      <c r="B269" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C269" s="7"/>
@@ -10921,7 +10945,7 @@
       <c r="A270" s="7" t="s">
         <v>1090</v>
       </c>
-      <c r="B270" s="25" t="s">
+      <c r="B270" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C270" s="7"/>
@@ -10941,7 +10965,7 @@
       <c r="A271" s="7" t="s">
         <v>1091</v>
       </c>
-      <c r="B271" s="25" t="s">
+      <c r="B271" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C271" s="7"/>
@@ -10961,7 +10985,7 @@
       <c r="A272" s="7" t="s">
         <v>1092</v>
       </c>
-      <c r="B272" s="25" t="s">
+      <c r="B272" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C272" s="7"/>
@@ -10981,7 +11005,7 @@
       <c r="A273" s="7" t="s">
         <v>1093</v>
       </c>
-      <c r="B273" s="25" t="s">
+      <c r="B273" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C273" s="7"/>
@@ -11001,7 +11025,7 @@
       <c r="A274" s="7" t="s">
         <v>1094</v>
       </c>
-      <c r="B274" s="25" t="s">
+      <c r="B274" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C274" s="7"/>
@@ -11021,7 +11045,7 @@
       <c r="A275" s="7" t="s">
         <v>1095</v>
       </c>
-      <c r="B275" s="25" t="s">
+      <c r="B275" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C275" s="7"/>
@@ -11041,7 +11065,7 @@
       <c r="A276" s="7" t="s">
         <v>1096</v>
       </c>
-      <c r="B276" s="25" t="s">
+      <c r="B276" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C276" s="7"/>
@@ -11061,7 +11085,7 @@
       <c r="A277" s="7" t="s">
         <v>1097</v>
       </c>
-      <c r="B277" s="25" t="s">
+      <c r="B277" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C277" s="7"/>
@@ -11081,7 +11105,7 @@
       <c r="A278" s="7" t="s">
         <v>1098</v>
       </c>
-      <c r="B278" s="25" t="s">
+      <c r="B278" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C278" s="7"/>
@@ -11101,7 +11125,7 @@
       <c r="A279" s="7" t="s">
         <v>1099</v>
       </c>
-      <c r="B279" s="25" t="s">
+      <c r="B279" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C279" s="7"/>
@@ -11121,7 +11145,7 @@
       <c r="A280" s="7" t="s">
         <v>1100</v>
       </c>
-      <c r="B280" s="25" t="s">
+      <c r="B280" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C280" s="7"/>
@@ -11141,7 +11165,7 @@
       <c r="A281" s="7" t="s">
         <v>1101</v>
       </c>
-      <c r="B281" s="25" t="s">
+      <c r="B281" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C281" s="7"/>
@@ -11161,7 +11185,7 @@
       <c r="A282" s="7" t="s">
         <v>1102</v>
       </c>
-      <c r="B282" s="25" t="s">
+      <c r="B282" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C282" s="7"/>
@@ -11181,7 +11205,7 @@
       <c r="A283" s="7" t="s">
         <v>1103</v>
       </c>
-      <c r="B283" s="25" t="s">
+      <c r="B283" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C283" s="7"/>
@@ -11201,7 +11225,7 @@
       <c r="A284" s="7" t="s">
         <v>1104</v>
       </c>
-      <c r="B284" s="25" t="s">
+      <c r="B284" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C284" s="7"/>
@@ -11221,7 +11245,7 @@
       <c r="A285" s="7" t="s">
         <v>1105</v>
       </c>
-      <c r="B285" s="25" t="s">
+      <c r="B285" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C285" s="7"/>
@@ -11241,7 +11265,7 @@
       <c r="A286" s="7" t="s">
         <v>1106</v>
       </c>
-      <c r="B286" s="25" t="s">
+      <c r="B286" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C286" s="7"/>
@@ -11261,7 +11285,7 @@
       <c r="A287" s="7" t="s">
         <v>1107</v>
       </c>
-      <c r="B287" s="25" t="s">
+      <c r="B287" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C287" s="7"/>
@@ -11281,7 +11305,7 @@
       <c r="A288" s="7" t="s">
         <v>1108</v>
       </c>
-      <c r="B288" s="25" t="s">
+      <c r="B288" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C288" s="7"/>
@@ -11301,7 +11325,7 @@
       <c r="A289" s="7" t="s">
         <v>1109</v>
       </c>
-      <c r="B289" s="25" t="s">
+      <c r="B289" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C289" s="7"/>
@@ -11321,7 +11345,7 @@
       <c r="A290" s="7" t="s">
         <v>1110</v>
       </c>
-      <c r="B290" s="25" t="s">
+      <c r="B290" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C290" s="7"/>
@@ -11341,7 +11365,7 @@
       <c r="A291" s="7" t="s">
         <v>1111</v>
       </c>
-      <c r="B291" s="25" t="s">
+      <c r="B291" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C291" s="7"/>
@@ -11361,7 +11385,7 @@
       <c r="A292" s="7" t="s">
         <v>1112</v>
       </c>
-      <c r="B292" s="25" t="s">
+      <c r="B292" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C292" s="7"/>
@@ -11381,7 +11405,7 @@
       <c r="A293" s="7" t="s">
         <v>1113</v>
       </c>
-      <c r="B293" s="25" t="s">
+      <c r="B293" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C293" s="7"/>
@@ -11401,7 +11425,7 @@
       <c r="A294" s="7" t="s">
         <v>1114</v>
       </c>
-      <c r="B294" s="25" t="s">
+      <c r="B294" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C294" s="7"/>
@@ -11421,7 +11445,7 @@
       <c r="A295" s="7" t="s">
         <v>1115</v>
       </c>
-      <c r="B295" s="25" t="s">
+      <c r="B295" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C295" s="7"/>
@@ -11441,7 +11465,7 @@
       <c r="A296" s="7" t="s">
         <v>1116</v>
       </c>
-      <c r="B296" s="25" t="s">
+      <c r="B296" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C296" s="7"/>
@@ -11461,7 +11485,7 @@
       <c r="A297" s="7" t="s">
         <v>1117</v>
       </c>
-      <c r="B297" s="25" t="s">
+      <c r="B297" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C297" s="7"/>
@@ -11481,7 +11505,7 @@
       <c r="A298" s="7" t="s">
         <v>1118</v>
       </c>
-      <c r="B298" s="25" t="s">
+      <c r="B298" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C298" s="7"/>
@@ -11501,7 +11525,7 @@
       <c r="A299" s="7" t="s">
         <v>1119</v>
       </c>
-      <c r="B299" s="25" t="s">
+      <c r="B299" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C299" s="7"/>
@@ -11521,7 +11545,7 @@
       <c r="A300" s="7" t="s">
         <v>1120</v>
       </c>
-      <c r="B300" s="25" t="s">
+      <c r="B300" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C300" s="7"/>
@@ -11541,7 +11565,7 @@
       <c r="A301" s="7" t="s">
         <v>1121</v>
       </c>
-      <c r="B301" s="25" t="s">
+      <c r="B301" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C301" s="7"/>
@@ -11561,7 +11585,7 @@
       <c r="A302" s="7" t="s">
         <v>1122</v>
       </c>
-      <c r="B302" s="25" t="s">
+      <c r="B302" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C302" s="7"/>
@@ -11581,7 +11605,7 @@
       <c r="A303" s="7" t="s">
         <v>1123</v>
       </c>
-      <c r="B303" s="25" t="s">
+      <c r="B303" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C303" s="7"/>
@@ -11601,7 +11625,7 @@
       <c r="A304" s="7" t="s">
         <v>1124</v>
       </c>
-      <c r="B304" s="25" t="s">
+      <c r="B304" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C304" s="7"/>
@@ -11621,7 +11645,7 @@
       <c r="A305" s="7" t="s">
         <v>1125</v>
       </c>
-      <c r="B305" s="25" t="s">
+      <c r="B305" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C305" s="7"/>
@@ -11641,7 +11665,7 @@
       <c r="A306" s="7" t="s">
         <v>1126</v>
       </c>
-      <c r="B306" s="25" t="s">
+      <c r="B306" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C306" s="7"/>
@@ -11661,7 +11685,7 @@
       <c r="A307" s="7" t="s">
         <v>1127</v>
       </c>
-      <c r="B307" s="25" t="s">
+      <c r="B307" s="28" t="s">
         <v>1041</v>
       </c>
       <c r="C307" s="7"/>

</xml_diff>